<commit_message>
Add links of interest spreadsheet
</commit_message>
<xml_diff>
--- a/Links of Interest about R.xlsx
+++ b/Links of Interest about R.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://american0-my.sharepoint.com/personal/janewall_american_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Awesome\OneDrive - american.edu\STAT412612\data_STAT412612\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="11_1D912C66B5C218EDD84EE64804297607C1FE3F77" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FA083B3-7538-4E48-A32E-63699BE9ACE2}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="11_1D912C66B5C218EDD84EE64804297607C1FE3F77" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{20041075-59B1-40DD-97BC-B37E5BE22989}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39280" yWindow="10830" windowWidth="16260" windowHeight="10690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -702,23 +702,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.86328125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="87.85546875" customWidth="1"/>
+    <col min="3" max="3" width="87.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -726,7 +726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>61</v>
       </c>
@@ -734,7 +734,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>107</v>
       </c>
@@ -742,7 +742,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>85</v>
       </c>
@@ -750,7 +750,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>86</v>
       </c>
@@ -758,7 +758,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>28</v>
       </c>
@@ -766,7 +766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>59</v>
       </c>
@@ -774,7 +774,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>63</v>
       </c>
@@ -782,7 +782,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>37</v>
       </c>
@@ -790,7 +790,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>45</v>
       </c>
@@ -798,7 +798,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>78</v>
       </c>
@@ -806,7 +806,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>49</v>
       </c>
@@ -814,12 +814,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>4</v>
       </c>
@@ -835,7 +835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -843,7 +843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -851,7 +851,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -859,7 +859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -867,7 +867,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>17</v>
       </c>
@@ -875,7 +875,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -883,7 +883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>30</v>
       </c>
@@ -891,7 +891,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>66</v>
       </c>
@@ -899,7 +899,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>68</v>
       </c>
@@ -907,7 +907,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>51</v>
       </c>
@@ -915,7 +915,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>84</v>
       </c>
@@ -923,12 +923,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>9</v>
       </c>
@@ -936,7 +936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>91</v>
       </c>
@@ -944,7 +944,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>104</v>
       </c>
@@ -952,7 +952,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>92</v>
       </c>
@@ -960,7 +960,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>57</v>
       </c>
@@ -968,7 +968,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>94</v>
       </c>
@@ -976,7 +976,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>76</v>
       </c>
@@ -984,12 +984,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>82</v>
       </c>
@@ -997,7 +997,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
         <v>72</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>74</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
         <v>54</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>55</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
         <v>5</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
         <v>7</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
         <v>70</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
         <v>70</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
         <v>21</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
         <v>32</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
         <v>24</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
         <v>26</v>
       </c>
@@ -1099,7 +1099,7 @@
     <hyperlink ref="C46" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C31" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="C17" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C18" r:id="rId5" location="dropbox" display="https://shiny.rstudio.com/articles/persistent-data-storage.html - dropbox" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C18" r:id="rId5" location="dropbox" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="C19" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="C21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="C22" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
@@ -1124,7 +1124,7 @@
     <hyperlink ref="C9" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="C5" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="C24" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C25" r:id="rId30" location="pre-workshop-set-up" display="https://happygitwithr.com/workshops.html - pre-workshop-set-up" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C25" r:id="rId30" location="pre-workshop-set-up" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
     <hyperlink ref="C47" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="C41" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="C42" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
@@ -1154,13 +1154,13 @@
       <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.59765625" customWidth="1"/>
+    <col min="2" max="2" width="69.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -1176,10 +1176,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>98</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>101</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
upload dataset for dates module
</commit_message>
<xml_diff>
--- a/Links of Interest about R.xlsx
+++ b/Links of Interest about R.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Awesome\OneDrive - american.edu\STAT412612\data_STAT412612\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://american0-my.sharepoint.com/personal/janewall_american_edu/Documents/STAT412612/data_STAT412612/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="11_1D912C66B5C218EDD84EE64804297607C1FE3F77" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{20041075-59B1-40DD-97BC-B37E5BE22989}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="11_1D912C66B5C218EDD84EE64804297607C1FE3F77" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{31C53FBA-6C80-4F42-94F1-283AAFD7E4D5}"/>
   <bookViews>
-    <workbookView xWindow="39280" yWindow="10830" windowWidth="16260" windowHeight="10690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
   <si>
     <t>https://www.r-bloggers.com/tidyquant-bringing-quantitative-financial-analysis-to-the-tidyverse/</t>
   </si>
@@ -356,6 +356,15 @@
   </si>
   <si>
     <t>More advanced topics</t>
+  </si>
+  <si>
+    <t>https://hansjoerg.me/2020/02/09/tidymodels-for-machine-learning/</t>
+  </si>
+  <si>
+    <t>https://www.tmwr.org/</t>
+  </si>
+  <si>
+    <t>Kuhn and Silge book Tidy Modeling with R</t>
   </si>
 </sst>
 </file>
@@ -700,25 +709,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.86328125" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="87.86328125" customWidth="1"/>
+    <col min="3" max="3" width="87.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -726,7 +735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>61</v>
       </c>
@@ -734,7 +743,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>107</v>
       </c>
@@ -742,7 +751,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>85</v>
       </c>
@@ -750,7 +759,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>86</v>
       </c>
@@ -758,7 +767,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>28</v>
       </c>
@@ -766,7 +775,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>59</v>
       </c>
@@ -774,7 +783,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>63</v>
       </c>
@@ -782,7 +791,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>37</v>
       </c>
@@ -790,7 +799,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>45</v>
       </c>
@@ -798,7 +807,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>78</v>
       </c>
@@ -806,7 +815,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>49</v>
       </c>
@@ -814,12 +823,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -827,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>4</v>
       </c>
@@ -835,7 +844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -843,7 +852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -851,7 +860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -859,7 +868,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -867,7 +876,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>17</v>
       </c>
@@ -875,7 +884,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -883,7 +892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>30</v>
       </c>
@@ -891,7 +900,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>66</v>
       </c>
@@ -899,7 +908,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>68</v>
       </c>
@@ -907,7 +916,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>51</v>
       </c>
@@ -915,7 +924,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>84</v>
       </c>
@@ -923,12 +932,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>9</v>
       </c>
@@ -936,7 +945,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>91</v>
       </c>
@@ -944,7 +953,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>104</v>
       </c>
@@ -952,7 +961,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>92</v>
       </c>
@@ -960,7 +969,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>57</v>
       </c>
@@ -968,7 +977,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>94</v>
       </c>
@@ -976,7 +985,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>76</v>
       </c>
@@ -984,139 +993,152 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B40" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B41" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B42" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B43" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B44" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B45" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B46" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B47" t="s">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B48" t="s">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>70</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B49" t="s">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>21</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B50" t="s">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B51" t="s">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>24</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B52" t="s">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C46" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C48" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C31" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="C17" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="C18" r:id="rId5" location="dropbox" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="C19" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="C21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="C22" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C49" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C51" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="C2" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C51" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C52" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C53" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C54" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="C7" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="C23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C50" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C45" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C52" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C47" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="C10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="C11" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="C13" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="C26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C43" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C44" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C45" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C46" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="C35" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="C8" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="C15" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
@@ -1125,14 +1147,14 @@
     <hyperlink ref="C5" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="C24" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
     <hyperlink ref="C25" r:id="rId30" location="pre-workshop-set-up" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C47" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C41" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C42" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C49" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C43" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C44" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
     <hyperlink ref="C37" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
     <hyperlink ref="C12" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C48" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C50" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
     <hyperlink ref="C20" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C42" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
     <hyperlink ref="C28" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
     <hyperlink ref="C6" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
     <hyperlink ref="C32" r:id="rId41" xr:uid="{9E5AC695-D72E-4A4C-AF08-948D4BB30AE7}"/>
@@ -1154,13 +1176,13 @@
       <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.59765625" customWidth="1"/>
-    <col min="2" max="2" width="69.59765625" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="69.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -1168,7 +1190,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -1176,10 +1198,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>98</v>
       </c>
@@ -1187,7 +1209,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>101</v>
       </c>
@@ -1195,7 +1217,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1203,7 +1225,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1211,7 +1233,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1219,7 +1241,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1227,7 +1249,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>

</xml_diff>